<commit_message>
Excel : reverting Y axis (put (0, 0) at bottom-left instead of top-left)
</commit_message>
<xml_diff>
--- a/models/model.xlsx
+++ b/models/model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="2">
   <si>
     <t>X</t>
   </si>
@@ -367,9 +367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -399,9 +397,7 @@
     </row>
     <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -418,7 +414,9 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
@@ -427,7 +425,9 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -475,7 +475,9 @@
       <c r="M4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -492,19 +494,29 @@
         <v>0</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,18 +529,26 @@
         <v>0</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N6" s="1"/>
+      <c r="N6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
@@ -541,7 +561,9 @@
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1" t="s">
         <v>0</v>
@@ -551,8 +573,12 @@
     </row>
     <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -568,81 +594,117 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N8" s="1"/>
-      <c r="O8" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -651,12 +713,18 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -667,30 +735,54 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -701,8 +793,12 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="O15" s="1"/>
     </row>
   </sheetData>

</xml_diff>